<commit_message>
Update and add speech analysis result spreadsheets
Updated MRMR speech analysis Excel files for both MFCCs and noMFCCs (sillabe and vocali). Added new results.xlsx and results_sillabe.xlsx files to the Results directory.
</commit_message>
<xml_diff>
--- a/Results/MRMR/Speech/noMFCCs/speech_noMFCCs_sillabe.xlsx
+++ b/Results/MRMR/Speech/noMFCCs/speech_noMFCCs_sillabe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1060,6 +1060,4131 @@
         <v>0.6666666666666666</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>{'C': 0.1, 'degree': 2, 'gamma': 1, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p']</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.6923076923076923</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 2, 'min_samples_split': 5, 'n_estimators': 100}</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p']</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>9</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.987012987012987</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 1.0, 'max_depth': 3, 'n_estimators': 40, 'subsample': 0.5}</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p']</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8</v>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>{'metric': 'euclidean', 'n_neighbors': 10, 'weights': 'distance'}</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p']</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>7</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" t="n">
+        <v>7</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (16,), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p']</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.6075949367088608</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>{'C': 20, 'degree': 2, 'gamma': 0.0001, 'kernel': 'linear'}</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k']</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>9</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.7435897435897436</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 1, 'min_samples_split': 5, 'n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k']</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.8421052631578947</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.5, 'max_depth': 2, 'n_estimators': 200, 'subsample': 0.5}</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k']</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.8421052631578947</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>{'metric': 'euclidean', 'n_neighbors': 5, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k']</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>7</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.7714285714285715</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (64,), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k']</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
+      <c r="F21" t="n">
+        <v>4</v>
+      </c>
+      <c r="G21" t="n">
+        <v>6</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.7088607594936709</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>{'C': 10, 'degree': 2, 'gamma': 0.001, 'kernel': 'rbf'}</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p']</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>6</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>10</v>
+      </c>
+      <c r="H22" t="n">
+        <v>4</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.7532467532467533</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 1, 'min_samples_split': 5, 'n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p']</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>5</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>10</v>
+      </c>
+      <c r="H23" t="n">
+        <v>5</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.2, 'max_depth': 2, 'n_estimators': 200, 'subsample': 0.5}</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p']</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>8</v>
+      </c>
+      <c r="F24" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" t="n">
+        <v>8</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 8, 'weights': 'distance'}</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p']</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>6</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3</v>
+      </c>
+      <c r="G25" t="n">
+        <v>7</v>
+      </c>
+      <c r="H25" t="n">
+        <v>4</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.631578947368421</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (32,), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p']</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>8</v>
+      </c>
+      <c r="F26" t="n">
+        <v>9</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.5925925925925926</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.4705882352941176</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>{'C': 0.1, 'degree': 2, 'gamma': 0.1, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k']</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>7</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" t="n">
+        <v>9</v>
+      </c>
+      <c r="H27" t="n">
+        <v>3</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.6753246753246753</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 4, 'min_samples_split': 2, 'n_estimators': 40}</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k']</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>8</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" t="n">
+        <v>8</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.5, 'max_depth': 2, 'n_estimators': 10, 'subsample': 0.2}</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k']</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>6</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="n">
+        <v>8</v>
+      </c>
+      <c r="H29" t="n">
+        <v>4</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.7848101265822784</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 15, 'weights': 'distance'}</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k']</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>7</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>10</v>
+      </c>
+      <c r="H30" t="n">
+        <v>3</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.8235294117647058</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (32,), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k']</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>7</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" t="n">
+        <v>8</v>
+      </c>
+      <c r="H31" t="n">
+        <v>3</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.704225352112676</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>{'C': 10, 'degree': 2, 'gamma': 0.0001, 'kernel': 'rbf'}</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p']</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>6</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>9</v>
+      </c>
+      <c r="H32" t="n">
+        <v>4</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.6376811594202898</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 4, 'min_samples_split': 10, 'n_estimators': 20}</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p']</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>7</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" t="n">
+        <v>9</v>
+      </c>
+      <c r="H33" t="n">
+        <v>3</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.9113924050632911</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.7, 'max_depth': 3, 'n_estimators': 100, 'subsample': 0.7}</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p']</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>6</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
+        <v>9</v>
+      </c>
+      <c r="H34" t="n">
+        <v>4</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 7, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p']</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>7</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" t="n">
+        <v>8</v>
+      </c>
+      <c r="H35" t="n">
+        <v>3</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.6944444444444444</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (64, 32), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p']</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>6</v>
+      </c>
+      <c r="F36" t="n">
+        <v>4</v>
+      </c>
+      <c r="G36" t="n">
+        <v>6</v>
+      </c>
+      <c r="H36" t="n">
+        <v>4</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0.7710843373493976</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>{'C': 0.2, 'degree': 2, 'gamma': 0.01, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k']</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>6</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="n">
+        <v>9</v>
+      </c>
+      <c r="H37" t="n">
+        <v>4</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0.676056338028169</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 2, 'min_samples_split': 2, 'n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k']</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>8</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" t="n">
+        <v>9</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.8421052631578947</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0.8947368421052632</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.5, 'max_depth': 2, 'n_estimators': 30, 'subsample': 0.7}</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k']</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>6</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>9</v>
+      </c>
+      <c r="H39" t="n">
+        <v>4</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 15, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k']</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>6</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>10</v>
+      </c>
+      <c r="H40" t="n">
+        <v>4</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L40" t="n">
+        <v>1</v>
+      </c>
+      <c r="M40" t="n">
+        <v>1</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0.704225352112676</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (32,), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k']</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>9</v>
+      </c>
+      <c r="F41" t="n">
+        <v>8</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.5294117647058824</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0.6428571428571429</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>{'C': 2, 'degree': 2, 'gamma': 0.01, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k']</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>7</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" t="n">
+        <v>9</v>
+      </c>
+      <c r="H42" t="n">
+        <v>3</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.7567567567567568</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 4, 'min_samples_split': 2, 'n_estimators': 20}</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k']</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>7</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" t="n">
+        <v>9</v>
+      </c>
+      <c r="H43" t="n">
+        <v>3</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.9459459459459459</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.2, 'max_depth': 2, 'n_estimators': 30, 'subsample': 0.2}</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k']</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>8</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" t="n">
+        <v>9</v>
+      </c>
+      <c r="H44" t="n">
+        <v>2</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.8421052631578947</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.7567567567567568</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 4, 'weights': 'distance'}</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k']</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>7</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2</v>
+      </c>
+      <c r="G45" t="n">
+        <v>8</v>
+      </c>
+      <c r="H45" t="n">
+        <v>3</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (16, 8), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k']</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>10</v>
+      </c>
+      <c r="F46" t="n">
+        <v>10</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K46" t="n">
+        <v>1</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>1</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>{'C': 1, 'degree': 2, 'gamma': 0.01, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t']</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>6</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" t="n">
+        <v>9</v>
+      </c>
+      <c r="H47" t="n">
+        <v>4</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0.7272727272727273</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 2, 'min_samples_split': 2, 'n_estimators': 100}</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t']</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>6</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" t="n">
+        <v>9</v>
+      </c>
+      <c r="H48" t="n">
+        <v>4</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.5, 'max_depth': 2, 'n_estimators': 40, 'subsample': 0.1}</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t']</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>9</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>8</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0.8181818181818182</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0.7848101265822784</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 15, 'weights': 'distance'}</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t']</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>6</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>10</v>
+      </c>
+      <c r="H50" t="n">
+        <v>4</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L50" t="n">
+        <v>1</v>
+      </c>
+      <c r="M50" t="n">
+        <v>1</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (32, 16), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t']</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>7</v>
+      </c>
+      <c r="F51" t="n">
+        <v>9</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" t="n">
+        <v>3</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.5384615384615384</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0.6732673267326733</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>{'C': 1, 'degree': 2, 'gamma': 0.01, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k']</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>6</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="n">
+        <v>9</v>
+      </c>
+      <c r="H52" t="n">
+        <v>4</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0.7341772151898734</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 2, 'min_samples_split': 2, 'n_estimators': 40}</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k']</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>7</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" t="n">
+        <v>9</v>
+      </c>
+      <c r="H53" t="n">
+        <v>3</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0.9866666666666667</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 20, 'subsample': 0.5}</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k']</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>6</v>
+      </c>
+      <c r="F54" t="n">
+        <v>2</v>
+      </c>
+      <c r="G54" t="n">
+        <v>8</v>
+      </c>
+      <c r="H54" t="n">
+        <v>4</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0.9473684210526315</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>{'metric': 'euclidean', 'n_neighbors': 15, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k']</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>6</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" t="n">
+        <v>9</v>
+      </c>
+      <c r="H55" t="n">
+        <v>4</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0.7027027027027027</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (16,), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k']</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>9</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" t="n">
+        <v>9</v>
+      </c>
+      <c r="H56" t="n">
+        <v>1</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0.7441860465116279</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>{'C': 1, 'degree': 2, 'gamma': 0.01, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k']</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>6</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" t="n">
+        <v>9</v>
+      </c>
+      <c r="H57" t="n">
+        <v>4</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0.775</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 2, 'min_samples_split': 2, 'n_estimators': 20}</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k']</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>5</v>
+      </c>
+      <c r="F58" t="n">
+        <v>2</v>
+      </c>
+      <c r="G58" t="n">
+        <v>8</v>
+      </c>
+      <c r="H58" t="n">
+        <v>5</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0.9866666666666667</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.5, 'max_depth': 2, 'n_estimators': 20, 'subsample': 0.3}</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k']</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>5</v>
+      </c>
+      <c r="F59" t="n">
+        <v>2</v>
+      </c>
+      <c r="G59" t="n">
+        <v>8</v>
+      </c>
+      <c r="H59" t="n">
+        <v>5</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0.7714285714285715</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 10, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k']</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>7</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" t="n">
+        <v>9</v>
+      </c>
+      <c r="H60" t="n">
+        <v>3</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (32,), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k']</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>8</v>
+      </c>
+      <c r="F61" t="n">
+        <v>8</v>
+      </c>
+      <c r="G61" t="n">
+        <v>2</v>
+      </c>
+      <c r="H61" t="n">
+        <v>2</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.6153846153846154</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0.6476190476190476</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>{'C': 0.0001, 'degree': 3, 'gamma': 0.1, 'kernel': 'poly'}</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t']</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>9</v>
+      </c>
+      <c r="F62" t="n">
+        <v>9</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O62" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 2, 'min_samples_split': 10, 'n_estimators': 20}</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t']</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>7</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" t="n">
+        <v>9</v>
+      </c>
+      <c r="H63" t="n">
+        <v>3</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0.9444444444444444</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.1, 'max_depth': 2, 'n_estimators': 30, 'subsample': 0.2}</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t']</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>7</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G64" t="n">
+        <v>9</v>
+      </c>
+      <c r="H64" t="n">
+        <v>3</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O64" t="n">
+        <v>0.7733333333333333</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 15, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t']</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>6</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" t="n">
+        <v>9</v>
+      </c>
+      <c r="H65" t="n">
+        <v>4</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O65" t="n">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (16,), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t']</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>9</v>
+      </c>
+      <c r="F66" t="n">
+        <v>2</v>
+      </c>
+      <c r="G66" t="n">
+        <v>8</v>
+      </c>
+      <c r="H66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0.8181818181818182</v>
+      </c>
+      <c r="M66" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O66" t="n">
+        <v>0.6265060240963856</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>{'C': 1, 'degree': 2, 'gamma': 0.01, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k']</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>6</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" t="n">
+        <v>9</v>
+      </c>
+      <c r="H67" t="n">
+        <v>4</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O67" t="n">
+        <v>0.7341772151898734</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 4, 'min_samples_split': 2, 'n_estimators': 30}</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k']</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>8</v>
+      </c>
+      <c r="F68" t="n">
+        <v>2</v>
+      </c>
+      <c r="G68" t="n">
+        <v>8</v>
+      </c>
+      <c r="H68" t="n">
+        <v>2</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M68" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O68" t="n">
+        <v>0.972972972972973</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.1, 'max_depth': 2, 'n_estimators': 30, 'subsample': 0.2}</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k']</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>7</v>
+      </c>
+      <c r="F69" t="n">
+        <v>1</v>
+      </c>
+      <c r="G69" t="n">
+        <v>9</v>
+      </c>
+      <c r="H69" t="n">
+        <v>3</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O69" t="n">
+        <v>0.7733333333333333</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 9, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k']</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>7</v>
+      </c>
+      <c r="F70" t="n">
+        <v>3</v>
+      </c>
+      <c r="G70" t="n">
+        <v>7</v>
+      </c>
+      <c r="H70" t="n">
+        <v>3</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O70" t="n">
+        <v>0.7469879518072289</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (16, 8), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k']</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>3</v>
+      </c>
+      <c r="F71" t="n">
+        <v>2</v>
+      </c>
+      <c r="G71" t="n">
+        <v>8</v>
+      </c>
+      <c r="H71" t="n">
+        <v>7</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="O71" t="n">
+        <v>0.4927536231884058</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>{'C': 0.1, 'degree': 2, 'gamma': 0.1, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t']</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>5</v>
+      </c>
+      <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="n">
+        <v>9</v>
+      </c>
+      <c r="H72" t="n">
+        <v>5</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="M72" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O72" t="n">
+        <v>0.5974025974025974</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 1, 'min_samples_split': 10, 'n_estimators': 40}</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t']</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>7</v>
+      </c>
+      <c r="F73" t="n">
+        <v>2</v>
+      </c>
+      <c r="G73" t="n">
+        <v>8</v>
+      </c>
+      <c r="H73" t="n">
+        <v>3</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="M73" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N73" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O73" t="n">
+        <v>0.9866666666666667</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 40, 'subsample': 0.3}</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t']</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>7</v>
+      </c>
+      <c r="F74" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" t="n">
+        <v>9</v>
+      </c>
+      <c r="H74" t="n">
+        <v>3</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O74" t="n">
+        <v>0.8918918918918919</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 9, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t']</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>7</v>
+      </c>
+      <c r="F75" t="n">
+        <v>2</v>
+      </c>
+      <c r="G75" t="n">
+        <v>8</v>
+      </c>
+      <c r="H75" t="n">
+        <v>3</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="M75" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N75" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O75" t="n">
+        <v>0.7619047619047619</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (8,), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t']</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>8</v>
+      </c>
+      <c r="F76" t="n">
+        <v>4</v>
+      </c>
+      <c r="G76" t="n">
+        <v>6</v>
+      </c>
+      <c r="H76" t="n">
+        <v>2</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L76" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="M76" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O76" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>{'C': 1, 'degree': 2, 'gamma': 0.01, 'kernel': 'sigmoid'}</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t']</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>6</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" t="n">
+        <v>9</v>
+      </c>
+      <c r="H77" t="n">
+        <v>4</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O77" t="n">
+        <v>0.7341772151898734</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 2, 'min_samples_split': 5, 'n_estimators': 20}</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t']</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>7</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G78" t="n">
+        <v>9</v>
+      </c>
+      <c r="H78" t="n">
+        <v>3</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L78" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M78" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N78" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O78" t="n">
+        <v>0.9866666666666667</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 200, 'subsample': 0.5}</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t']</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>8</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>10</v>
+      </c>
+      <c r="H79" t="n">
+        <v>2</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L79" t="n">
+        <v>1</v>
+      </c>
+      <c r="M79" t="n">
+        <v>1</v>
+      </c>
+      <c r="N79" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 9, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t']</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>6</v>
+      </c>
+      <c r="F80" t="n">
+        <v>2</v>
+      </c>
+      <c r="G80" t="n">
+        <v>8</v>
+      </c>
+      <c r="H80" t="n">
+        <v>4</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L80" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M80" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N80" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O80" t="n">
+        <v>0.7435897435897436</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (32, 16), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t']</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>7</v>
+      </c>
+      <c r="F81" t="n">
+        <v>7</v>
+      </c>
+      <c r="G81" t="n">
+        <v>3</v>
+      </c>
+      <c r="H81" t="n">
+        <v>3</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L81" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M81" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N81" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O81" t="n">
+        <v>0.6788990825688074</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>{'C': 20, 'degree': 4, 'gamma': 0.01, 'kernel': 'poly'}</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t', 'f3_min_k', 'EnergyBurst_p', 'jitter_local_k', 'HFLFRatio_k', 'f0_25_p']</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>6</v>
+      </c>
+      <c r="F82" t="n">
+        <v>6</v>
+      </c>
+      <c r="G82" t="n">
+        <v>4</v>
+      </c>
+      <c r="H82" t="n">
+        <v>4</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0.5454545454545454</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L82" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M82" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N82" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O82" t="n">
+        <v>0.8941176470588236</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>{'max_depth': None, 'min_samples_leaf': 1, 'min_samples_split': 5, 'n_estimators': 60}</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t', 'f3_min_k', 'EnergyBurst_p', 'jitter_local_k', 'HFLFRatio_k', 'f0_25_p']</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>6</v>
+      </c>
+      <c r="F83" t="n">
+        <v>1</v>
+      </c>
+      <c r="G83" t="n">
+        <v>9</v>
+      </c>
+      <c r="H83" t="n">
+        <v>4</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L83" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M83" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N83" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>XGB</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.1, 'max_depth': 5, 'n_estimators': 30, 'subsample': 0.5}</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t', 'f3_min_k', 'EnergyBurst_p', 'jitter_local_k', 'HFLFRatio_k', 'f0_25_p']</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>7</v>
+      </c>
+      <c r="F84" t="n">
+        <v>1</v>
+      </c>
+      <c r="G84" t="n">
+        <v>9</v>
+      </c>
+      <c r="H84" t="n">
+        <v>3</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L84" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M84" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N84" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O84" t="n">
+        <v>0.9736842105263158</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>{'metric': 'manhattan', 'n_neighbors': 15, 'weights': 'distance'}</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t', 'f3_min_k', 'EnergyBurst_p', 'jitter_local_k', 'HFLFRatio_k', 'f0_25_p']</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>6</v>
+      </c>
+      <c r="F85" t="n">
+        <v>1</v>
+      </c>
+      <c r="G85" t="n">
+        <v>9</v>
+      </c>
+      <c r="H85" t="n">
+        <v>4</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L85" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M85" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N85" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MLP</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (16, 8), 'learning_rate': 'constant'}</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>['duration_k', 'f3_median_t', 'f0_75_k', 'tot_articulation_p', 'shimmer_apq11_p', 'tot_articulation_t', 'duration_p', 'EnergyDrop_p', 'tot_articulation_k', 'f0_median_k', 'f2_min_k', 'duration_t', 'number_of repetitons_t', 'jitter_local_absolute_k', 'number_of repetitons_p', 'low_energy_p', 'f0_mean_k', 'f1_min_p', 'number_of repetitons_k', 'f2_mean_k', 'low_energy_t', 'f0_std_k', 'f1_mean_p', 'EnergyBurst_k', 'VOT_p', 'f2_min_t', 'hnr_std_k', 'MaxBurstAmplitude_dB_p', 'VOT_t', 'f2_median_k', 'f1_mean_k', 'f0_std_t', 'low_energy_k', 'PeakFreq_t', 'f0_max_k', 'f3_min_t', 'f0_25_k', 'f1_std_p', 'f0_std_p', 'f0_75_t', 'hnr_min_p', 'f3_std_p', 'f1_median_p', 'MaxBurstAmplitude_dB_k', 'f1_min_k', 'hnr_std_p', 'f0_75_p', 'f3_min_p', 'f1_median_k', 'EnergyDrop_k', 'f1_min_t', 'hnr_max_k', 'shimmer_local_dB_p', 'EnergyDrop_t', 'f0_median_t', 'shimmer_local_p', 'VarFreq_p', 'f3_max_p', 'f0_max_p', 'f2_std_k', 'MaxBurstAmplitude_dB_t', 'f0_median_p', 'f3_max_k', 'MeanFreq_t', 'cpp_t', 'f0_mean_p', 'f2_min_p', 'hnr_min_t', 'cpp_k', 'f1_mean_t', 'f3_min_k', 'EnergyBurst_p', 'jitter_local_k', 'HFLFRatio_k', 'f0_25_p']</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>9</v>
+      </c>
+      <c r="F86" t="n">
+        <v>9</v>
+      </c>
+      <c r="G86" t="n">
+        <v>1</v>
+      </c>
+      <c r="H86" t="n">
+        <v>1</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L86" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M86" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N86" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O86" t="n">
+        <v>0.6548672566371682</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>